<commit_message>
Added more model data
</commit_message>
<xml_diff>
--- a/design/Mental Model.xlsx
+++ b/design/Mental Model.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="67">
   <si>
     <t>View product details</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Basket[]</t>
   </si>
   <si>
-    <t>Log in to account</t>
-  </si>
-  <si>
     <t>Nice to have</t>
   </si>
   <si>
@@ -97,13 +94,136 @@
   </si>
   <si>
     <t>Card details</t>
+  </si>
+  <si>
+    <t>Add Product to Wishlist</t>
+  </si>
+  <si>
+    <t>Wishlist[]</t>
+  </si>
+  <si>
+    <t>Log in to existing account or create new account</t>
+  </si>
+  <si>
+    <t>Save details in account</t>
+  </si>
+  <si>
+    <t>Add product to account wishlist</t>
+  </si>
+  <si>
+    <t>Log in to existing account</t>
+  </si>
+  <si>
+    <t>View wishlist</t>
+  </si>
+  <si>
+    <t>AddToWishlist()</t>
+  </si>
+  <si>
+    <t>View and Update Wishlist</t>
+  </si>
+  <si>
+    <t>Adjust product quantity</t>
+  </si>
+  <si>
+    <t>Adjust product priority</t>
+  </si>
+  <si>
+    <t>Remove product from wishlist</t>
+  </si>
+  <si>
+    <t>RemoveFromWishlist()</t>
+  </si>
+  <si>
+    <t>Search products</t>
+  </si>
+  <si>
+    <t>Search()</t>
+  </si>
+  <si>
+    <t>Quick-view product details</t>
+  </si>
+  <si>
+    <t>QuickViewProduct()</t>
+  </si>
+  <si>
+    <t>Register New Account</t>
+  </si>
+  <si>
+    <t>Enter email address</t>
+  </si>
+  <si>
+    <t>Enter password</t>
+  </si>
+  <si>
+    <t>Confirm password</t>
+  </si>
+  <si>
+    <t>Enter name</t>
+  </si>
+  <si>
+    <t>Enter correspondence address</t>
+  </si>
+  <si>
+    <t>Confirm catalogue preference</t>
+  </si>
+  <si>
+    <t>Complete registration</t>
+  </si>
+  <si>
+    <t>Accept terms and conditions</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>Register</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>addressline1</t>
+  </si>
+  <si>
+    <t>addressline2</t>
+  </si>
+  <si>
+    <t>addressline3</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>county</t>
+  </si>
+  <si>
+    <t>postal_code</t>
+  </si>
+  <si>
+    <t>send_catalogue</t>
+  </si>
+  <si>
+    <t>t&amp;cs_accepted</t>
+  </si>
+  <si>
+    <t>CreateAccount()</t>
+  </si>
+  <si>
+    <t>Login to Account</t>
+  </si>
+  <si>
+    <t>Confirm login</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,6 +242,14 @@
     <font>
       <sz val="11"/>
       <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -153,7 +281,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -213,11 +341,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -246,20 +385,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -562,166 +713,344 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R17"/>
+  <dimension ref="A1:AX21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2.85546875" style="1"/>
-    <col min="3" max="5" width="14.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="2.85546875" style="1"/>
-    <col min="7" max="7" width="1.42578125" style="1" customWidth="1"/>
+    <col min="3" max="7" width="14.28515625" style="1" customWidth="1"/>
     <col min="8" max="8" width="2.85546875" style="1"/>
-    <col min="9" max="16" width="14.28515625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="2.85546875" style="1"/>
-    <col min="18" max="18" width="1.42578125" style="1" customWidth="1"/>
-    <col min="19" max="16384" width="2.85546875" style="1"/>
+    <col min="9" max="9" width="1.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="2.85546875" style="1"/>
+    <col min="11" max="19" width="14.28515625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="2.85546875" style="1"/>
+    <col min="21" max="21" width="1.42578125" style="1" customWidth="1"/>
+    <col min="22" max="22" width="2.85546875" style="1"/>
+    <col min="23" max="24" width="14.28515625" style="1" customWidth="1"/>
+    <col min="25" max="25" width="2.85546875" style="1"/>
+    <col min="26" max="26" width="1.42578125" style="1" customWidth="1"/>
+    <col min="27" max="27" width="2.85546875" style="1"/>
+    <col min="28" max="33" width="14.28515625" style="1" customWidth="1"/>
+    <col min="34" max="34" width="2.85546875" style="1"/>
+    <col min="35" max="35" width="1.42578125" style="1" customWidth="1"/>
+    <col min="36" max="36" width="2.85546875" style="1"/>
+    <col min="37" max="44" width="14.28515625" style="1" customWidth="1"/>
+    <col min="45" max="45" width="2.85546875" style="1"/>
+    <col min="46" max="46" width="1.42578125" style="1" customWidth="1"/>
+    <col min="47" max="47" width="2.85546875" style="1"/>
+    <col min="48" max="50" width="14.28515625" style="1" customWidth="1"/>
+    <col min="51" max="16384" width="2.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="G1" s="2"/>
-      <c r="R1" s="2"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C2" s="6" t="s">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="I1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="Z1" s="2"/>
+      <c r="AI1" s="2"/>
+      <c r="AT1" s="2"/>
+    </row>
+    <row r="2" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="G2" s="2"/>
-      <c r="I2" s="6" t="s">
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="6"/>
+      <c r="I2" s="2"/>
+      <c r="K2" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-      <c r="R2" s="2"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="G3" s="2"/>
-      <c r="R3" s="2"/>
-    </row>
-    <row r="4" spans="1:18" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="7" t="s">
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16"/>
+      <c r="S2" s="16"/>
+      <c r="U2" s="2"/>
+      <c r="W2" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="X2" s="16"/>
+      <c r="Z2" s="2"/>
+      <c r="AB2" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC2" s="16"/>
+      <c r="AD2" s="16"/>
+      <c r="AE2" s="16"/>
+      <c r="AF2" s="16"/>
+      <c r="AG2" s="6"/>
+      <c r="AI2" s="2"/>
+      <c r="AK2" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="AL2" s="16"/>
+      <c r="AM2" s="16"/>
+      <c r="AN2" s="16"/>
+      <c r="AO2" s="16"/>
+      <c r="AP2" s="16"/>
+      <c r="AQ2" s="16"/>
+      <c r="AR2" s="16"/>
+      <c r="AT2" s="2"/>
+      <c r="AV2" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="AW2" s="16"/>
+      <c r="AX2" s="16"/>
+    </row>
+    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="I3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="Z3" s="2"/>
+      <c r="AI3" s="2"/>
+      <c r="AT3" s="2"/>
+    </row>
+    <row r="4" spans="1:50" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="3"/>
+      <c r="E4" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="I4" s="2"/>
+      <c r="K4" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="N4" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="O4" s="8"/>
+      <c r="P4" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q4" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="R4" s="8"/>
+      <c r="S4" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="U4" s="2"/>
+      <c r="W4" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="X4" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z4" s="2"/>
+      <c r="AB4" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC4" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF4" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG4" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI4" s="2"/>
+      <c r="AK4" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="AL4" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="AR4" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="AT4" s="2"/>
+      <c r="AV4" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="AW4" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="AX4" s="13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:50" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="I4" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="K4" s="7" t="s">
+      <c r="I5" s="2"/>
+      <c r="K5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="13"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="13"/>
+      <c r="U5" s="2"/>
+      <c r="W5" s="13"/>
+      <c r="X5" s="13"/>
+      <c r="Z5" s="2"/>
+      <c r="AB5" s="13"/>
+      <c r="AC5" s="13"/>
+      <c r="AF5" s="13"/>
+      <c r="AG5" s="13"/>
+      <c r="AI5" s="2"/>
+      <c r="AK5" s="13"/>
+      <c r="AL5" s="13"/>
+      <c r="AM5" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO5" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="AQ5" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="AR5" s="13"/>
+      <c r="AT5" s="2"/>
+      <c r="AV5" s="13"/>
+      <c r="AW5" s="13"/>
+      <c r="AX5" s="13"/>
+    </row>
+    <row r="6" spans="1:50" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="I6" s="2"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="M4" s="8"/>
-      <c r="N4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="O4" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="P4" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="R4" s="2"/>
-    </row>
-    <row r="5" spans="1:18" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="G5" s="2"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-      <c r="R5" s="2"/>
-    </row>
-    <row r="6" spans="1:18" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="G6" s="2"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="10" t="s">
+      <c r="M6" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="N6" s="13"/>
+      <c r="O6" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="8"/>
+      <c r="S6" s="13"/>
+      <c r="U6" s="2"/>
+      <c r="W6" s="13"/>
+      <c r="X6" s="13"/>
+      <c r="Z6" s="2"/>
+      <c r="AB6" s="13"/>
+      <c r="AC6" s="13"/>
+      <c r="AD6" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF6" s="13"/>
+      <c r="AG6" s="13"/>
+      <c r="AI6" s="2"/>
+      <c r="AK6" s="13"/>
+      <c r="AL6" s="13"/>
+      <c r="AM6" s="13"/>
+      <c r="AO6" s="13"/>
+      <c r="AQ6" s="13"/>
+      <c r="AR6" s="13"/>
+      <c r="AT6" s="2"/>
+      <c r="AV6" s="13"/>
+      <c r="AW6" s="13"/>
+      <c r="AX6" s="13"/>
+    </row>
+    <row r="7" spans="1:50" s="10" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
-      <c r="R6" s="2"/>
-    </row>
-    <row r="7" spans="1:18" s="11" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="G7" s="12"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="I7" s="11"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="15"/>
       <c r="M7" s="13"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="R7" s="12"/>
-    </row>
-    <row r="8" spans="1:18" s="2" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G9" s="4"/>
-      <c r="R9" s="4"/>
-    </row>
-    <row r="10" spans="1:18" s="3" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N7" s="13"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="13"/>
+      <c r="R7" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="S7" s="13"/>
+      <c r="U7" s="11"/>
+      <c r="W7" s="13"/>
+      <c r="X7" s="13"/>
+      <c r="Z7" s="11"/>
+      <c r="AB7" s="13"/>
+      <c r="AC7" s="13"/>
+      <c r="AD7" s="13"/>
+      <c r="AE7" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF7" s="13"/>
+      <c r="AG7" s="13"/>
+      <c r="AI7" s="11"/>
+      <c r="AK7" s="13"/>
+      <c r="AL7" s="13"/>
+      <c r="AM7" s="13"/>
+      <c r="AN7" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="AO7" s="13"/>
+      <c r="AP7" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="AQ7" s="13"/>
+      <c r="AR7" s="13"/>
+      <c r="AT7" s="11"/>
+      <c r="AV7" s="13"/>
+      <c r="AW7" s="13"/>
+      <c r="AX7" s="13"/>
+    </row>
+    <row r="8" spans="1:50" s="2" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:50" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I9" s="4"/>
+      <c r="U9" s="4"/>
+      <c r="Z9" s="4"/>
+      <c r="AI9" s="4"/>
+      <c r="AT9" s="4"/>
+    </row>
+    <row r="10" spans="1:50" s="3" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="D10" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G10" s="4"/>
-      <c r="I10" s="5" t="s">
+      <c r="G10" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="J10" s="5" t="s">
-        <v>15</v>
-      </c>
+      <c r="I10" s="4"/>
       <c r="K10" s="5" t="s">
         <v>15</v>
       </c>
@@ -729,89 +1058,320 @@
         <v>15</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="N10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="O10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="P10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q10" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="O10" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="P10" s="5" t="s">
+      <c r="R10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="S10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="R10" s="4"/>
-    </row>
-    <row r="11" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G11" s="4"/>
-      <c r="R11" s="4"/>
-    </row>
-    <row r="12" spans="1:18" s="3" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U10" s="4"/>
+      <c r="W10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="X10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z10" s="4"/>
+      <c r="AB10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="AC10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="AD10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="AF10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="AG10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="AI10" s="4"/>
+      <c r="AK10" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="AL10" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM10" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN10" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="AO10" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="AP10" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="AQ10" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="AR10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="AT10" s="4"/>
+      <c r="AV10" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="AW10" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="AX10" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:50" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I11" s="4"/>
+      <c r="U11" s="4"/>
+      <c r="Z11" s="4"/>
+      <c r="AI11" s="4"/>
+      <c r="AT11" s="4"/>
+    </row>
+    <row r="12" spans="1:50" s="3" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="D12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I12" s="4"/>
+      <c r="K12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="O12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q12" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="R12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="S12" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="4"/>
-      <c r="I12" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="J12" s="5" t="s">
+      <c r="U12" s="4"/>
+      <c r="W12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="X12" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z12" s="4"/>
+      <c r="AB12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="AC12" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD12" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE12" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF12" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG12" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="AI12" s="4"/>
+      <c r="AO12" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="AR12" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="AT12" s="4"/>
+      <c r="AX12" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:50" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I13" s="4"/>
+      <c r="U13" s="4"/>
+      <c r="Z13" s="4"/>
+      <c r="AI13" s="4"/>
+      <c r="AK13" s="1"/>
+      <c r="AL13" s="1"/>
+      <c r="AM13" s="1"/>
+      <c r="AN13" s="1"/>
+      <c r="AO13" s="1"/>
+      <c r="AP13" s="1"/>
+      <c r="AQ13" s="1"/>
+      <c r="AT13" s="4"/>
+    </row>
+    <row r="14" spans="1:50" s="3" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D14" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="I14" s="4"/>
+      <c r="O14" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="R14" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="S14" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="U14" s="4"/>
+      <c r="W14" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="X14" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z14" s="4"/>
+      <c r="AF14" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="AG14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="AI14" s="4"/>
+      <c r="AK14" s="1"/>
+      <c r="AL14" s="1"/>
+      <c r="AM14" s="1"/>
+      <c r="AN14" s="1"/>
+      <c r="AO14" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="AP14" s="1"/>
+      <c r="AQ14" s="1"/>
+      <c r="AT14" s="4"/>
+    </row>
+    <row r="15" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="I15" s="2"/>
+      <c r="U15" s="2"/>
+      <c r="Z15" s="2"/>
+      <c r="AG15" s="3"/>
+      <c r="AI15" s="2"/>
+      <c r="AT15" s="2"/>
+    </row>
+    <row r="16" spans="1:50" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I16" s="2"/>
+      <c r="S16" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="U16" s="2"/>
+      <c r="Z16" s="2"/>
+      <c r="AG16" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="M12" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="O12" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="P12" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="R12" s="4"/>
-    </row>
-    <row r="13" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G13" s="4"/>
-      <c r="R13" s="4"/>
-    </row>
-    <row r="14" spans="1:18" s="3" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G14" s="4"/>
-      <c r="P14" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="R14" s="4"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="G15" s="2"/>
-      <c r="R15" s="2"/>
-    </row>
-    <row r="16" spans="1:18" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G16" s="2"/>
-      <c r="P16" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="R16" s="2"/>
-    </row>
-    <row r="17" spans="7:18" x14ac:dyDescent="0.25">
-      <c r="G17" s="2"/>
-      <c r="R17" s="2"/>
+      <c r="AI16" s="2"/>
+      <c r="AO16" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="AT16" s="2"/>
+    </row>
+    <row r="17" spans="9:46" x14ac:dyDescent="0.25">
+      <c r="I17" s="2"/>
+      <c r="U17" s="2"/>
+      <c r="Z17" s="2"/>
+      <c r="AI17" s="2"/>
+      <c r="AT17" s="2"/>
+    </row>
+    <row r="18" spans="9:46" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I18" s="2"/>
+      <c r="U18" s="2"/>
+      <c r="Z18" s="2"/>
+      <c r="AI18" s="2"/>
+      <c r="AO18" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="AT18" s="2"/>
+    </row>
+    <row r="19" spans="9:46" x14ac:dyDescent="0.25">
+      <c r="I19" s="2"/>
+      <c r="U19" s="2"/>
+      <c r="Z19" s="2"/>
+      <c r="AI19" s="2"/>
+      <c r="AT19" s="2"/>
+    </row>
+    <row r="20" spans="9:46" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I20" s="2"/>
+      <c r="U20" s="2"/>
+      <c r="Z20" s="2"/>
+      <c r="AI20" s="2"/>
+      <c r="AO20" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="AT20" s="2"/>
+    </row>
+    <row r="21" spans="9:46" x14ac:dyDescent="0.25">
+      <c r="I21" s="2"/>
+      <c r="U21" s="2"/>
+      <c r="Z21" s="2"/>
+      <c r="AI21" s="2"/>
+      <c r="AT21" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="I4:I7"/>
+  <mergeCells count="34">
+    <mergeCell ref="AK2:AR2"/>
+    <mergeCell ref="AX4:AX7"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="AV4:AV7"/>
+    <mergeCell ref="AV2:AX2"/>
+    <mergeCell ref="AG4:AG7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="AR4:AR7"/>
+    <mergeCell ref="AQ5:AQ7"/>
+    <mergeCell ref="AO5:AO7"/>
+    <mergeCell ref="AM5:AM7"/>
+    <mergeCell ref="AL4:AL7"/>
+    <mergeCell ref="AK4:AK7"/>
+    <mergeCell ref="AF4:AF7"/>
+    <mergeCell ref="AD6:AD7"/>
     <mergeCell ref="M6:M7"/>
-    <mergeCell ref="I2:P2"/>
-    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="AB2:AF2"/>
+    <mergeCell ref="X4:X7"/>
+    <mergeCell ref="W4:W7"/>
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="AC4:AC7"/>
+    <mergeCell ref="AB4:AB7"/>
+    <mergeCell ref="O6:O7"/>
+    <mergeCell ref="C2:F2"/>
     <mergeCell ref="E4:E7"/>
-    <mergeCell ref="D4:D7"/>
     <mergeCell ref="C4:C7"/>
+    <mergeCell ref="S4:S7"/>
+    <mergeCell ref="Q4:Q7"/>
     <mergeCell ref="P4:P7"/>
-    <mergeCell ref="O4:O7"/>
     <mergeCell ref="N4:N7"/>
-    <mergeCell ref="L4:L7"/>
     <mergeCell ref="K4:K7"/>
-    <mergeCell ref="J4:J7"/>
+    <mergeCell ref="K2:S2"/>
+    <mergeCell ref="L6:L7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>